<commit_message>
merge solutions for tuples & triples in local embd search
</commit_message>
<xml_diff>
--- a/output/frat/conceptnet-local_embedding_search/depth_1/frat_2,3_conceptnet_search.xlsx
+++ b/output/frat/conceptnet-local_embedding_search/depth_1/frat_2,3_conceptnet_search.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="10808"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="24228"/>
   <workbookPr defaultThemeVersion="124226"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/rejna/projects/github.com/r_m_thesis/output/frat/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\projects\r_m_thesis\output\frat\conceptnet-local_embedding_search\depth_1\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C6038DC6-0341-0A4E-8715-106A6526B3D7}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DA61A1B6-AF71-4123-A974-076E88771639}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="240" yWindow="500" windowWidth="28560" windowHeight="17500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="4560" yWindow="4560" windowWidth="28800" windowHeight="15560" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -1899,20 +1899,24 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:I194"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A54" workbookViewId="0">
-      <selection activeCell="E76" sqref="E76"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="E174" sqref="E174"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultColWidth="8.81640625" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="1" max="1" width="22.33203125" customWidth="1"/>
-    <col min="2" max="2" width="28.6640625" customWidth="1"/>
-    <col min="3" max="3" width="24.83203125" customWidth="1"/>
-    <col min="4" max="4" width="26.5" customWidth="1"/>
-    <col min="5" max="5" width="46.1640625" customWidth="1"/>
+    <col min="1" max="1" width="22.36328125" customWidth="1"/>
+    <col min="2" max="2" width="28.6328125" customWidth="1"/>
+    <col min="3" max="3" width="24.81640625" customWidth="1"/>
+    <col min="4" max="4" width="26.453125" customWidth="1"/>
+    <col min="5" max="5" width="46.1796875" customWidth="1"/>
+    <col min="6" max="6" width="13.81640625" customWidth="1"/>
+    <col min="7" max="7" width="22.453125" customWidth="1"/>
+    <col min="8" max="8" width="36.26953125" customWidth="1"/>
+    <col min="9" max="9" width="29.90625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -1941,7 +1945,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="2" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A2" t="s">
         <v>9</v>
       </c>
@@ -1964,7 +1968,7 @@
         <v>422</v>
       </c>
     </row>
-    <row r="3" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A3" t="s">
         <v>10</v>
       </c>
@@ -1987,7 +1991,7 @@
         <v>423</v>
       </c>
     </row>
-    <row r="4" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A4" t="s">
         <v>11</v>
       </c>
@@ -2010,7 +2014,7 @@
         <v>424</v>
       </c>
     </row>
-    <row r="5" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A5" t="s">
         <v>12</v>
       </c>
@@ -2033,7 +2037,7 @@
         <v>425</v>
       </c>
     </row>
-    <row r="6" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A6" t="s">
         <v>13</v>
       </c>
@@ -2047,7 +2051,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="7" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A7" t="s">
         <v>14</v>
       </c>
@@ -2061,7 +2065,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="8" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="8" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A8" t="s">
         <v>15</v>
       </c>
@@ -2084,7 +2088,7 @@
         <v>426</v>
       </c>
     </row>
-    <row r="9" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="9" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A9" t="s">
         <v>16</v>
       </c>
@@ -2098,7 +2102,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="10" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="10" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A10" t="s">
         <v>17</v>
       </c>
@@ -2121,7 +2125,7 @@
         <v>427</v>
       </c>
     </row>
-    <row r="11" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="11" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A11" t="s">
         <v>18</v>
       </c>
@@ -2144,7 +2148,7 @@
         <v>428</v>
       </c>
     </row>
-    <row r="12" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="12" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A12" t="s">
         <v>19</v>
       </c>
@@ -2167,7 +2171,7 @@
         <v>429</v>
       </c>
     </row>
-    <row r="13" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="13" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A13" t="s">
         <v>20</v>
       </c>
@@ -2190,7 +2194,7 @@
         <v>430</v>
       </c>
     </row>
-    <row r="14" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="14" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A14" t="s">
         <v>21</v>
       </c>
@@ -2213,7 +2217,7 @@
         <v>431</v>
       </c>
     </row>
-    <row r="15" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="15" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A15" t="s">
         <v>22</v>
       </c>
@@ -2236,7 +2240,7 @@
         <v>432</v>
       </c>
     </row>
-    <row r="16" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="16" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A16" t="s">
         <v>23</v>
       </c>
@@ -2259,7 +2263,7 @@
         <v>433</v>
       </c>
     </row>
-    <row r="17" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="17" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A17" t="s">
         <v>24</v>
       </c>
@@ -2282,7 +2286,7 @@
         <v>434</v>
       </c>
     </row>
-    <row r="18" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="18" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A18" t="s">
         <v>25</v>
       </c>
@@ -2305,7 +2309,7 @@
         <v>435</v>
       </c>
     </row>
-    <row r="19" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="19" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A19" t="s">
         <v>26</v>
       </c>
@@ -2328,7 +2332,7 @@
         <v>436</v>
       </c>
     </row>
-    <row r="20" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="20" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A20" t="s">
         <v>27</v>
       </c>
@@ -2351,7 +2355,7 @@
         <v>437</v>
       </c>
     </row>
-    <row r="21" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="21" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A21" t="s">
         <v>28</v>
       </c>
@@ -2374,7 +2378,7 @@
         <v>438</v>
       </c>
     </row>
-    <row r="22" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="22" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A22" t="s">
         <v>29</v>
       </c>
@@ -2388,7 +2392,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="23" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="23" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A23" t="s">
         <v>30</v>
       </c>
@@ -2411,7 +2415,7 @@
         <v>439</v>
       </c>
     </row>
-    <row r="24" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="24" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A24" t="s">
         <v>31</v>
       </c>
@@ -2425,7 +2429,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="25" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="25" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A25" t="s">
         <v>32</v>
       </c>
@@ -2439,7 +2443,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="26" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="26" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A26" t="s">
         <v>33</v>
       </c>
@@ -2462,7 +2466,7 @@
         <v>440</v>
       </c>
     </row>
-    <row r="27" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="27" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A27" t="s">
         <v>34</v>
       </c>
@@ -2479,7 +2483,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="28" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="28" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A28" t="s">
         <v>35</v>
       </c>
@@ -2496,7 +2500,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="29" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="29" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A29" t="s">
         <v>36</v>
       </c>
@@ -2513,7 +2517,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="30" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="30" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A30" t="s">
         <v>37</v>
       </c>
@@ -2530,7 +2534,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="31" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="31" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A31" t="s">
         <v>38</v>
       </c>
@@ -2544,7 +2548,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="32" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="32" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A32" t="s">
         <v>39</v>
       </c>
@@ -2567,7 +2571,7 @@
         <v>441</v>
       </c>
     </row>
-    <row r="33" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="33" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A33" t="s">
         <v>40</v>
       </c>
@@ -2581,7 +2585,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="34" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="34" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A34" t="s">
         <v>41</v>
       </c>
@@ -2598,7 +2602,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="35" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="35" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A35" t="s">
         <v>42</v>
       </c>
@@ -2612,7 +2616,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="36" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="36" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A36" t="s">
         <v>43</v>
       </c>
@@ -2635,7 +2639,7 @@
         <v>442</v>
       </c>
     </row>
-    <row r="37" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="37" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A37" t="s">
         <v>44</v>
       </c>
@@ -2649,7 +2653,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="38" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="38" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A38" t="s">
         <v>45</v>
       </c>
@@ -2672,7 +2676,7 @@
         <v>443</v>
       </c>
     </row>
-    <row r="39" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="39" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A39" t="s">
         <v>46</v>
       </c>
@@ -2689,7 +2693,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="40" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="40" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A40" t="s">
         <v>47</v>
       </c>
@@ -2706,7 +2710,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="41" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="41" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A41" t="s">
         <v>48</v>
       </c>
@@ -2720,7 +2724,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="42" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="42" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A42" t="s">
         <v>49</v>
       </c>
@@ -2743,7 +2747,7 @@
         <v>444</v>
       </c>
     </row>
-    <row r="43" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="43" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A43" t="s">
         <v>50</v>
       </c>
@@ -2766,7 +2770,7 @@
         <v>445</v>
       </c>
     </row>
-    <row r="44" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="44" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A44" t="s">
         <v>51</v>
       </c>
@@ -2789,7 +2793,7 @@
         <v>446</v>
       </c>
     </row>
-    <row r="45" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="45" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A45" t="s">
         <v>52</v>
       </c>
@@ -2812,7 +2816,7 @@
         <v>447</v>
       </c>
     </row>
-    <row r="46" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="46" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A46" t="s">
         <v>53</v>
       </c>
@@ -2835,7 +2839,7 @@
         <v>448</v>
       </c>
     </row>
-    <row r="47" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="47" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A47" t="s">
         <v>54</v>
       </c>
@@ -2858,7 +2862,7 @@
         <v>449</v>
       </c>
     </row>
-    <row r="48" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="48" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A48" t="s">
         <v>55</v>
       </c>
@@ -2881,7 +2885,7 @@
         <v>450</v>
       </c>
     </row>
-    <row r="49" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="49" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A49" t="s">
         <v>56</v>
       </c>
@@ -2904,7 +2908,7 @@
         <v>451</v>
       </c>
     </row>
-    <row r="50" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="50" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A50" t="s">
         <v>57</v>
       </c>
@@ -2918,7 +2922,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="51" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="51" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A51" t="s">
         <v>58</v>
       </c>
@@ -2935,7 +2939,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="52" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="52" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A52" t="s">
         <v>59</v>
       </c>
@@ -2958,7 +2962,7 @@
         <v>452</v>
       </c>
     </row>
-    <row r="53" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="53" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A53" t="s">
         <v>60</v>
       </c>
@@ -2972,7 +2976,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="54" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="54" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A54" t="s">
         <v>61</v>
       </c>
@@ -2995,7 +2999,7 @@
         <v>453</v>
       </c>
     </row>
-    <row r="55" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="55" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A55" t="s">
         <v>62</v>
       </c>
@@ -3018,7 +3022,7 @@
         <v>454</v>
       </c>
     </row>
-    <row r="56" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="56" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A56" t="s">
         <v>63</v>
       </c>
@@ -3041,7 +3045,7 @@
         <v>455</v>
       </c>
     </row>
-    <row r="57" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="57" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A57" t="s">
         <v>64</v>
       </c>
@@ -3064,7 +3068,7 @@
         <v>456</v>
       </c>
     </row>
-    <row r="58" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="58" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A58" t="s">
         <v>65</v>
       </c>
@@ -3081,7 +3085,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="59" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="59" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A59" t="s">
         <v>66</v>
       </c>
@@ -3098,7 +3102,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="60" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="60" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A60" t="s">
         <v>67</v>
       </c>
@@ -3121,7 +3125,7 @@
         <v>457</v>
       </c>
     </row>
-    <row r="61" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="61" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A61" t="s">
         <v>68</v>
       </c>
@@ -3138,7 +3142,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="62" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="62" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A62" t="s">
         <v>69</v>
       </c>
@@ -3161,7 +3165,7 @@
         <v>458</v>
       </c>
     </row>
-    <row r="63" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="63" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A63" t="s">
         <v>70</v>
       </c>
@@ -3184,7 +3188,7 @@
         <v>459</v>
       </c>
     </row>
-    <row r="64" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="64" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A64" t="s">
         <v>71</v>
       </c>
@@ -3207,7 +3211,7 @@
         <v>460</v>
       </c>
     </row>
-    <row r="65" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="65" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A65" t="s">
         <v>72</v>
       </c>
@@ -3230,7 +3234,7 @@
         <v>461</v>
       </c>
     </row>
-    <row r="66" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="66" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A66" t="s">
         <v>73</v>
       </c>
@@ -3247,7 +3251,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="67" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="67" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A67" t="s">
         <v>74</v>
       </c>
@@ -3270,7 +3274,7 @@
         <v>462</v>
       </c>
     </row>
-    <row r="68" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="68" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A68" t="s">
         <v>75</v>
       </c>
@@ -3284,7 +3288,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="69" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="69" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A69" t="s">
         <v>76</v>
       </c>
@@ -3298,7 +3302,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="70" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="70" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A70" t="s">
         <v>77</v>
       </c>
@@ -3321,7 +3325,7 @@
         <v>463</v>
       </c>
     </row>
-    <row r="71" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="71" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A71" t="s">
         <v>78</v>
       </c>
@@ -3344,7 +3348,7 @@
         <v>464</v>
       </c>
     </row>
-    <row r="72" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="72" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A72" t="s">
         <v>79</v>
       </c>
@@ -3367,7 +3371,7 @@
         <v>465</v>
       </c>
     </row>
-    <row r="73" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="73" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A73" t="s">
         <v>80</v>
       </c>
@@ -3390,7 +3394,7 @@
         <v>466</v>
       </c>
     </row>
-    <row r="74" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="74" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A74" t="s">
         <v>81</v>
       </c>
@@ -3407,7 +3411,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="75" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="75" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A75" t="s">
         <v>82</v>
       </c>
@@ -3430,7 +3434,7 @@
         <v>467</v>
       </c>
     </row>
-    <row r="76" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="76" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A76" t="s">
         <v>83</v>
       </c>
@@ -3444,7 +3448,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="77" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="77" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A77" t="s">
         <v>84</v>
       </c>
@@ -3458,7 +3462,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="78" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="78" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A78" t="s">
         <v>85</v>
       </c>
@@ -3481,7 +3485,7 @@
         <v>468</v>
       </c>
     </row>
-    <row r="79" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="79" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A79" t="s">
         <v>86</v>
       </c>
@@ -3504,7 +3508,7 @@
         <v>469</v>
       </c>
     </row>
-    <row r="80" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="80" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A80" t="s">
         <v>87</v>
       </c>
@@ -3527,7 +3531,7 @@
         <v>470</v>
       </c>
     </row>
-    <row r="81" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="81" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A81" t="s">
         <v>88</v>
       </c>
@@ -3550,7 +3554,7 @@
         <v>471</v>
       </c>
     </row>
-    <row r="82" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="82" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A82" t="s">
         <v>89</v>
       </c>
@@ -3564,7 +3568,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="83" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="83" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A83" t="s">
         <v>90</v>
       </c>
@@ -3581,7 +3585,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="84" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="84" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A84" t="s">
         <v>91</v>
       </c>
@@ -3595,7 +3599,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="85" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="85" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A85" t="s">
         <v>92</v>
       </c>
@@ -3609,7 +3613,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="86" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="86" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A86" t="s">
         <v>93</v>
       </c>
@@ -3623,7 +3627,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="87" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="87" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A87" t="s">
         <v>94</v>
       </c>
@@ -3637,7 +3641,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="88" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="88" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A88" t="s">
         <v>95</v>
       </c>
@@ -3651,7 +3655,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="89" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="89" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A89" t="s">
         <v>96</v>
       </c>
@@ -3665,7 +3669,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="90" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="90" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A90" t="s">
         <v>97</v>
       </c>
@@ -3682,7 +3686,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="91" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="91" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A91" t="s">
         <v>98</v>
       </c>
@@ -3699,7 +3703,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="92" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="92" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A92" t="s">
         <v>99</v>
       </c>
@@ -3713,7 +3717,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="93" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="93" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A93" t="s">
         <v>100</v>
       </c>
@@ -3727,7 +3731,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="94" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="94" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A94" t="s">
         <v>101</v>
       </c>
@@ -3744,7 +3748,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="95" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="95" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A95" t="s">
         <v>102</v>
       </c>
@@ -3758,7 +3762,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="96" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="96" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A96" t="s">
         <v>103</v>
       </c>
@@ -3781,7 +3785,7 @@
         <v>472</v>
       </c>
     </row>
-    <row r="97" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="97" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A97" t="s">
         <v>104</v>
       </c>
@@ -3795,7 +3799,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="98" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="98" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A98" t="s">
         <v>105</v>
       </c>
@@ -3809,7 +3813,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="99" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="99" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A99" t="s">
         <v>106</v>
       </c>
@@ -3823,7 +3827,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="100" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="100" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A100" t="s">
         <v>107</v>
       </c>
@@ -3840,7 +3844,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="101" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="101" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A101" t="s">
         <v>108</v>
       </c>
@@ -3854,7 +3858,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="102" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="102" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A102" t="s">
         <v>109</v>
       </c>
@@ -3868,7 +3872,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="103" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="103" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A103" t="s">
         <v>110</v>
       </c>
@@ -3885,7 +3889,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="104" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="104" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A104" t="s">
         <v>111</v>
       </c>
@@ -3908,7 +3912,7 @@
         <v>473</v>
       </c>
     </row>
-    <row r="105" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="105" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A105" t="s">
         <v>112</v>
       </c>
@@ -3922,7 +3926,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="106" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="106" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A106" t="s">
         <v>113</v>
       </c>
@@ -3945,7 +3949,7 @@
         <v>474</v>
       </c>
     </row>
-    <row r="107" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="107" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A107" t="s">
         <v>114</v>
       </c>
@@ -3968,7 +3972,7 @@
         <v>475</v>
       </c>
     </row>
-    <row r="108" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="108" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A108" t="s">
         <v>115</v>
       </c>
@@ -3991,7 +3995,7 @@
         <v>476</v>
       </c>
     </row>
-    <row r="109" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="109" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A109" t="s">
         <v>116</v>
       </c>
@@ -4014,7 +4018,7 @@
         <v>477</v>
       </c>
     </row>
-    <row r="110" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="110" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A110" t="s">
         <v>117</v>
       </c>
@@ -4031,7 +4035,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="111" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="111" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A111" t="s">
         <v>118</v>
       </c>
@@ -4048,7 +4052,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="112" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="112" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A112" t="s">
         <v>119</v>
       </c>
@@ -4071,7 +4075,7 @@
         <v>478</v>
       </c>
     </row>
-    <row r="113" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="113" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A113" t="s">
         <v>120</v>
       </c>
@@ -4088,7 +4092,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="114" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="114" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A114" t="s">
         <v>121</v>
       </c>
@@ -4102,7 +4106,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="115" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="115" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A115" t="s">
         <v>122</v>
       </c>
@@ -4116,7 +4120,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="116" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="116" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A116" t="s">
         <v>123</v>
       </c>
@@ -4130,7 +4134,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="117" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="117" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A117" t="s">
         <v>124</v>
       </c>
@@ -4144,7 +4148,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="118" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="118" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A118" t="s">
         <v>125</v>
       </c>
@@ -4158,7 +4162,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="119" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="119" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A119" t="s">
         <v>126</v>
       </c>
@@ -4172,7 +4176,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="120" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="120" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A120" t="s">
         <v>127</v>
       </c>
@@ -4189,7 +4193,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="121" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="121" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A121" t="s">
         <v>128</v>
       </c>
@@ -4203,7 +4207,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="122" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="122" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A122" t="s">
         <v>129</v>
       </c>
@@ -4217,7 +4221,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="123" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="123" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A123" t="s">
         <v>130</v>
       </c>
@@ -4231,7 +4235,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="124" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="124" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A124" t="s">
         <v>131</v>
       </c>
@@ -4254,7 +4258,7 @@
         <v>479</v>
       </c>
     </row>
-    <row r="125" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="125" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A125" t="s">
         <v>132</v>
       </c>
@@ -4268,7 +4272,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="126" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="126" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A126" t="s">
         <v>133</v>
       </c>
@@ -4291,7 +4295,7 @@
         <v>480</v>
       </c>
     </row>
-    <row r="127" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="127" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A127" t="s">
         <v>134</v>
       </c>
@@ -4314,7 +4318,7 @@
         <v>481</v>
       </c>
     </row>
-    <row r="128" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="128" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A128" t="s">
         <v>135</v>
       </c>
@@ -4337,7 +4341,7 @@
         <v>482</v>
       </c>
     </row>
-    <row r="129" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="129" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A129" t="s">
         <v>136</v>
       </c>
@@ -4360,7 +4364,7 @@
         <v>483</v>
       </c>
     </row>
-    <row r="130" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="130" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A130" t="s">
         <v>137</v>
       </c>
@@ -4377,7 +4381,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="131" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="131" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A131" t="s">
         <v>138</v>
       </c>
@@ -4394,7 +4398,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="132" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="132" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A132" t="s">
         <v>139</v>
       </c>
@@ -4417,7 +4421,7 @@
         <v>484</v>
       </c>
     </row>
-    <row r="133" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="133" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A133" t="s">
         <v>140</v>
       </c>
@@ -4434,7 +4438,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="134" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="134" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A134" t="s">
         <v>141</v>
       </c>
@@ -4457,7 +4461,7 @@
         <v>485</v>
       </c>
     </row>
-    <row r="135" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="135" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A135" t="s">
         <v>142</v>
       </c>
@@ -4480,7 +4484,7 @@
         <v>486</v>
       </c>
     </row>
-    <row r="136" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="136" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A136" t="s">
         <v>143</v>
       </c>
@@ -4503,7 +4507,7 @@
         <v>487</v>
       </c>
     </row>
-    <row r="137" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="137" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A137" t="s">
         <v>144</v>
       </c>
@@ -4526,7 +4530,7 @@
         <v>488</v>
       </c>
     </row>
-    <row r="138" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="138" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A138" t="s">
         <v>145</v>
       </c>
@@ -4540,7 +4544,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="139" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="139" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A139" t="s">
         <v>146</v>
       </c>
@@ -4563,7 +4567,7 @@
         <v>489</v>
       </c>
     </row>
-    <row r="140" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="140" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A140" t="s">
         <v>147</v>
       </c>
@@ -4577,7 +4581,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="141" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="141" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A141" t="s">
         <v>148</v>
       </c>
@@ -4591,7 +4595,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="142" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="142" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A142" t="s">
         <v>149</v>
       </c>
@@ -4608,7 +4612,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="143" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="143" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A143" t="s">
         <v>150</v>
       </c>
@@ -4625,7 +4629,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="144" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="144" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A144" t="s">
         <v>151</v>
       </c>
@@ -4639,7 +4643,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="145" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="145" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A145" t="s">
         <v>152</v>
       </c>
@@ -4653,7 +4657,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="146" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="146" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A146" t="s">
         <v>153</v>
       </c>
@@ -4670,7 +4674,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="147" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="147" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A147" t="s">
         <v>154</v>
       </c>
@@ -4687,7 +4691,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="148" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="148" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A148" t="s">
         <v>155</v>
       </c>
@@ -4704,7 +4708,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="149" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="149" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A149" t="s">
         <v>156</v>
       </c>
@@ -4721,7 +4725,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="150" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="150" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A150" t="s">
         <v>157</v>
       </c>
@@ -4735,7 +4739,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="151" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="151" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A151" t="s">
         <v>158</v>
       </c>
@@ -4749,7 +4753,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="152" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="152" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A152" t="s">
         <v>159</v>
       </c>
@@ -4763,7 +4767,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="153" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="153" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A153" t="s">
         <v>160</v>
       </c>
@@ -4777,7 +4781,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="154" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="154" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A154" t="s">
         <v>161</v>
       </c>
@@ -4791,7 +4795,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="155" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="155" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A155" t="s">
         <v>162</v>
       </c>
@@ -4808,7 +4812,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="156" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="156" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A156" t="s">
         <v>163</v>
       </c>
@@ -4825,7 +4829,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="157" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="157" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A157" t="s">
         <v>164</v>
       </c>
@@ -4839,7 +4843,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="158" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="158" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A158" t="s">
         <v>165</v>
       </c>
@@ -4856,7 +4860,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="159" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="159" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A159" t="s">
         <v>166</v>
       </c>
@@ -4873,7 +4877,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="160" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="160" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A160" t="s">
         <v>167</v>
       </c>
@@ -4890,7 +4894,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="161" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="161" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A161" t="s">
         <v>168</v>
       </c>
@@ -4904,7 +4908,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="162" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="162" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A162" t="s">
         <v>169</v>
       </c>
@@ -4927,7 +4931,7 @@
         <v>490</v>
       </c>
     </row>
-    <row r="163" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="163" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A163" t="s">
         <v>170</v>
       </c>
@@ -4944,7 +4948,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="164" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="164" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A164" t="s">
         <v>171</v>
       </c>
@@ -4961,7 +4965,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="165" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="165" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A165" t="s">
         <v>172</v>
       </c>
@@ -4975,7 +4979,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="166" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="166" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A166" t="s">
         <v>173</v>
       </c>
@@ -4992,7 +4996,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="167" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="167" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A167" t="s">
         <v>174</v>
       </c>
@@ -5006,7 +5010,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="168" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="168" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A168" t="s">
         <v>175</v>
       </c>
@@ -5020,7 +5024,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="169" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="169" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A169" t="s">
         <v>176</v>
       </c>
@@ -5034,7 +5038,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="170" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="170" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A170" t="s">
         <v>177</v>
       </c>
@@ -5048,7 +5052,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="171" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="171" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A171" t="s">
         <v>178</v>
       </c>
@@ -5062,7 +5066,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="172" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="172" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A172" t="s">
         <v>179</v>
       </c>
@@ -5079,7 +5083,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="173" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="173" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A173" t="s">
         <v>180</v>
       </c>
@@ -5093,7 +5097,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="174" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="174" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A174" t="s">
         <v>181</v>
       </c>
@@ -5110,7 +5114,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="175" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="175" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A175" t="s">
         <v>182</v>
       </c>
@@ -5127,7 +5131,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="176" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="176" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A176" t="s">
         <v>183</v>
       </c>
@@ -5144,7 +5148,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="177" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="177" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A177" t="s">
         <v>184</v>
       </c>
@@ -5158,7 +5162,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="178" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="178" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A178" t="s">
         <v>185</v>
       </c>
@@ -5172,7 +5176,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="179" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="179" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A179" t="s">
         <v>186</v>
       </c>
@@ -5186,7 +5190,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="180" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="180" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A180" t="s">
         <v>187</v>
       </c>
@@ -5200,7 +5204,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="181" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="181" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A181" t="s">
         <v>188</v>
       </c>
@@ -5214,7 +5218,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="182" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="182" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A182" t="s">
         <v>189</v>
       </c>
@@ -5231,7 +5235,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="183" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="183" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A183" t="s">
         <v>190</v>
       </c>
@@ -5248,7 +5252,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="184" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="184" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A184" t="s">
         <v>191</v>
       </c>
@@ -5262,7 +5266,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="185" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="185" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A185" t="s">
         <v>192</v>
       </c>
@@ -5276,7 +5280,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="186" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="186" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A186" t="s">
         <v>193</v>
       </c>
@@ -5293,7 +5297,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="187" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="187" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A187" t="s">
         <v>194</v>
       </c>
@@ -5310,7 +5314,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="188" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="188" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A188" t="s">
         <v>195</v>
       </c>
@@ -5327,7 +5331,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="189" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="189" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A189" t="s">
         <v>196</v>
       </c>
@@ -5341,7 +5345,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="190" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="190" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A190" t="s">
         <v>197</v>
       </c>
@@ -5358,7 +5362,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="191" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="191" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A191" t="s">
         <v>198</v>
       </c>
@@ -5372,7 +5376,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="192" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="192" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A192" t="s">
         <v>199</v>
       </c>
@@ -5389,7 +5393,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="193" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="193" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A193" t="s">
         <v>200</v>
       </c>
@@ -5403,7 +5407,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="194" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="194" spans="1:9" x14ac:dyDescent="0.35">
       <c r="I194" t="s">
         <v>491</v>
       </c>

</xml_diff>